<commit_message>
Updated murine source spec to add death elements
</commit_message>
<xml_diff>
--- a/docs/ims/ims-metadata.xlsx
+++ b/docs/ims/ims-metadata.xlsx
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>version</t>
   </si>
@@ -1271,7 +1271,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from ms_source list." sqref="Q2:Q1048576">
-      <formula1>'ms_source list'!$A$1:$A$7</formula1>
+      <formula1>'ms_source list'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: negative ion mode / positive ion mode / negative and positive ion mode." sqref="R2:R1048576">
       <formula1>'polarity list'!$A$1:$A$3</formula1>
@@ -1503,7 +1503,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1541,6 +1541,11 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>